<commit_message>
Updated stats for twinbrook with new distances
</commit_message>
<xml_diff>
--- a/twinbrook_stats.xlsx
+++ b/twinbrook_stats.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e81612f1f3deee4b/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e81612f1f3deee4b/Documents/Project1SUMO/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="135" documentId="8_{FF337BD7-DE9A-46E6-AC74-BE6EB01D1D55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DD1FA7E3-8F15-4766-A5C3-34D96316B449}"/>
+  <xr:revisionPtr revIDLastSave="268" documentId="8_{FF337BD7-DE9A-46E6-AC74-BE6EB01D1D55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C54A6FBA-62D6-4581-AA5C-AA4B7F70738D}"/>
   <bookViews>
-    <workbookView xWindow="12750" yWindow="3990" windowWidth="28800" windowHeight="15435" xr2:uid="{6CABBCD2-87B3-48BA-BE7D-5CBDB21DB40C}"/>
+    <workbookView xWindow="870" yWindow="3945" windowWidth="28800" windowHeight="15435" xr2:uid="{6CABBCD2-87B3-48BA-BE7D-5CBDB21DB40C}"/>
   </bookViews>
   <sheets>
     <sheet name="Twinbrook Rd" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="35">
   <si>
     <t>twinbrook_detector_EB0</t>
   </si>
@@ -205,10 +205,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Calculation" xfId="1" builtinId="22"/>
@@ -527,7 +527,7 @@
   <dimension ref="A2:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,21 +549,21 @@
       <c r="A2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1" t="s">
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -635,73 +635,73 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>534.33333333333303</v>
       </c>
-      <c r="D5" s="2">
-        <v>36.243156643792801</v>
-      </c>
-      <c r="E5" s="2">
+      <c r="D5" s="1">
+        <v>29.2669398500936</v>
+      </c>
+      <c r="E5" s="1">
         <v>82.42</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <v>274.666666666666</v>
       </c>
-      <c r="G5" s="2">
-        <v>61.748978697504597</v>
-      </c>
-      <c r="H5" s="2">
+      <c r="G5" s="1">
+        <v>34.262582825822101</v>
+      </c>
+      <c r="H5" s="1">
         <v>59.84</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="1">
         <v>188.47200000000001</v>
       </c>
-      <c r="J5" s="2">
-        <v>62.660886034115002</v>
-      </c>
-      <c r="K5" s="2">
+      <c r="J5" s="1">
+        <v>33.126599569429402</v>
+      </c>
+      <c r="K5" s="1">
         <v>66.78</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>660.66666666666595</v>
       </c>
-      <c r="D6" s="2">
-        <v>26.735388944977199</v>
-      </c>
-      <c r="E6" s="2">
+      <c r="D6" s="1">
+        <v>26.3003068216271</v>
+      </c>
+      <c r="E6" s="1">
         <v>85.76</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <v>423.5</v>
       </c>
-      <c r="G6" s="2">
-        <v>52.917416489988199</v>
-      </c>
-      <c r="H6" s="2">
+      <c r="G6" s="1">
+        <v>51.415014296936299</v>
+      </c>
+      <c r="H6" s="1">
         <v>61.25</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="1">
         <v>294.61399999999998</v>
       </c>
-      <c r="J6" s="2">
-        <v>56.693057307953701</v>
-      </c>
-      <c r="K6" s="2">
+      <c r="J6" s="1">
+        <v>55.514835133287697</v>
+      </c>
+      <c r="K6" s="1">
         <v>67.430000000000007</v>
       </c>
     </row>
@@ -740,73 +740,73 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>338.666666666666</v>
       </c>
-      <c r="D8" s="2">
-        <v>52.175357380254198</v>
-      </c>
-      <c r="E8" s="2">
+      <c r="D8" s="1">
+        <v>46.070254260528898</v>
+      </c>
+      <c r="E8" s="1">
         <v>59.42</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="1">
         <v>431.166666666666</v>
       </c>
-      <c r="G8" s="2">
-        <v>70.335099499807598</v>
-      </c>
-      <c r="H8" s="2">
+      <c r="G8" s="1">
+        <v>56.138624095457999</v>
+      </c>
+      <c r="H8" s="1">
         <v>33.68</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="1">
         <v>854.774</v>
       </c>
-      <c r="J8" s="2">
-        <v>16.123031742940501</v>
-      </c>
-      <c r="K8" s="2">
+      <c r="J8" s="1">
+        <v>14.1038898837209</v>
+      </c>
+      <c r="K8" s="1">
         <v>63.2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+    <row r="9" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>242.666666666666</v>
       </c>
-      <c r="D9" s="2">
-        <v>74.773174166666607</v>
-      </c>
-      <c r="E9" s="2">
+      <c r="D9" s="1">
+        <v>59.897605292479099</v>
+      </c>
+      <c r="E9" s="1">
         <v>32.590000000000003</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="1">
         <v>175.5</v>
       </c>
-      <c r="G9" s="2">
-        <v>212.047981075888</v>
-      </c>
-      <c r="H9" s="2">
+      <c r="G9" s="1">
+        <v>187.68558105769199</v>
+      </c>
+      <c r="H9" s="1">
         <v>13.78</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="1">
         <v>326.74</v>
       </c>
-      <c r="J9" s="2">
-        <v>83.797384786885203</v>
-      </c>
-      <c r="K9" s="2">
+      <c r="J9" s="1">
+        <v>70.545204664031601</v>
+      </c>
+      <c r="K9" s="1">
         <v>22.09</v>
       </c>
     </row>
@@ -821,7 +821,7 @@
         <v>5</v>
       </c>
       <c r="D10">
-        <v>5634.1681857142803</v>
+        <v>5813.3583250000001</v>
       </c>
       <c r="E10">
         <v>0.51</v>
@@ -830,7 +830,7 @@
         <v>4.8333333333333304</v>
       </c>
       <c r="G10">
-        <v>7661.8577206896498</v>
+        <v>7588.7599821428503</v>
       </c>
       <c r="H10">
         <v>0.3</v>
@@ -839,7 +839,7 @@
         <v>4.66</v>
       </c>
       <c r="J10">
-        <v>5840.9233652173898</v>
+        <v>5589.2049904761898</v>
       </c>
       <c r="K10">
         <v>0.35</v>
@@ -856,7 +856,7 @@
         <v>6.3333333333333304</v>
       </c>
       <c r="D11">
-        <v>5164.1816444444403</v>
+        <v>4800.0823874999996</v>
       </c>
       <c r="E11">
         <v>0.25</v>
@@ -865,7 +865,7 @@
         <v>7.8333333333333304</v>
       </c>
       <c r="G11">
-        <v>4121.7017765957398</v>
+        <v>4480.2299326086904</v>
       </c>
       <c r="H11">
         <v>0.38</v>
@@ -874,7 +874,7 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="J11">
-        <v>4891.3021478260798</v>
+        <v>5025.5998954545403</v>
       </c>
       <c r="K11">
         <v>0.28999999999999998</v>
@@ -891,7 +891,7 @@
         <v>1</v>
       </c>
       <c r="D12">
-        <v>8230.1355999999996</v>
+        <v>4560.9952000000003</v>
       </c>
       <c r="E12">
         <v>0.09</v>
@@ -900,7 +900,7 @@
         <v>1</v>
       </c>
       <c r="G12">
-        <v>51927.2227666666</v>
+        <v>49732.808720000001</v>
       </c>
       <c r="H12">
         <v>0.11</v>
@@ -909,7 +909,7 @@
         <v>0.2</v>
       </c>
       <c r="J12">
-        <v>191443.99</v>
+        <v>205924.0526</v>
       </c>
       <c r="K12">
         <v>0</v>
@@ -926,7 +926,7 @@
         <v>4.6666666666666599</v>
       </c>
       <c r="D13">
-        <v>4936.8220230769202</v>
+        <v>4630.5787454545398</v>
       </c>
       <c r="E13">
         <v>0.73</v>
@@ -935,7 +935,7 @@
         <v>4.3333333333333304</v>
       </c>
       <c r="G13">
-        <v>7730.7719846153796</v>
+        <v>8365.4122839999909</v>
       </c>
       <c r="H13">
         <v>0.49</v>
@@ -944,7 +944,7 @@
         <v>2.6</v>
       </c>
       <c r="J13">
-        <v>8997.5732384615294</v>
+        <v>10547.5343333333</v>
       </c>
       <c r="K13">
         <v>0.55000000000000004</v>
@@ -954,21 +954,21 @@
       <c r="A15" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1" t="s">
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1" t="s">
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1005,67 +1005,367 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="1">
+        <v>503.33333333333297</v>
+      </c>
+      <c r="D18" s="1">
+        <v>48.092518205980099</v>
+      </c>
+      <c r="E18" s="1">
+        <v>68.62</v>
+      </c>
+      <c r="F18" s="1">
+        <v>283.5</v>
+      </c>
+      <c r="G18" s="1">
+        <v>58.259761429415001</v>
+      </c>
+      <c r="H18" s="1">
+        <v>57.49</v>
+      </c>
+      <c r="I18" s="1">
+        <v>253.75</v>
+      </c>
+      <c r="J18" s="1">
+        <v>49.128383201581002</v>
+      </c>
+      <c r="K18" s="1">
+        <v>72.48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="1">
+        <v>692</v>
+      </c>
+      <c r="D19" s="1">
+        <v>31.431881529581499</v>
+      </c>
+      <c r="E19" s="1">
+        <v>72.900000000000006</v>
+      </c>
+      <c r="F19" s="1">
+        <v>414.666666666666</v>
+      </c>
+      <c r="G19" s="1">
+        <v>51.5862726071285</v>
+      </c>
+      <c r="H19" s="1">
+        <v>58.43</v>
+      </c>
+      <c r="I19" s="1">
+        <v>348</v>
+      </c>
+      <c r="J19" s="1">
+        <v>49.866908106169198</v>
+      </c>
+      <c r="K19" s="1">
+        <v>72.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G20">
+        <v>133747.63080000001</v>
+      </c>
+      <c r="H20">
+        <v>0.03</v>
+      </c>
+      <c r="I20">
+        <v>0.25</v>
+      </c>
+      <c r="J20">
+        <v>131500.58979999999</v>
+      </c>
+      <c r="K20">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="B21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="1">
+        <v>480.666666666666</v>
+      </c>
+      <c r="D21" s="1">
+        <v>78.921944206896598</v>
+      </c>
+      <c r="E21" s="1">
+        <v>22.7</v>
+      </c>
+      <c r="F21" s="1">
+        <v>455.33333333333297</v>
+      </c>
+      <c r="G21" s="1">
+        <v>67.203411614317005</v>
+      </c>
+      <c r="H21" s="1">
+        <v>28.62</v>
+      </c>
+      <c r="I21" s="1">
+        <v>1044.25</v>
+      </c>
+      <c r="J21" s="1">
+        <v>34.663753187394697</v>
+      </c>
+      <c r="K21" s="1">
+        <v>29.19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="1">
+        <v>101.666666666666</v>
+      </c>
+      <c r="D22" s="1">
+        <v>357.77319050847399</v>
+      </c>
+      <c r="E22" s="1">
+        <v>6.11</v>
+      </c>
+      <c r="F22" s="1">
+        <v>151.333333333333</v>
+      </c>
+      <c r="G22" s="1">
+        <v>244.67948303769401</v>
+      </c>
+      <c r="H22" s="1">
+        <v>10.57</v>
+      </c>
+      <c r="I22" s="1">
+        <v>138.5</v>
+      </c>
+      <c r="J22" s="1">
+        <v>393.38181029668402</v>
+      </c>
+      <c r="K22" s="1">
+        <v>4.29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23">
+        <v>5</v>
+      </c>
+      <c r="D23">
+        <v>5825.2674857142802</v>
+      </c>
+      <c r="E23">
+        <v>0.4</v>
+      </c>
+      <c r="F23">
+        <v>4.8333333333333304</v>
+      </c>
+      <c r="G23">
+        <v>7420.9070344827496</v>
+      </c>
+      <c r="H23">
+        <v>0.24</v>
+      </c>
+      <c r="I23">
+        <v>5.25</v>
+      </c>
+      <c r="J23">
+        <v>6655.7124000000003</v>
+      </c>
+      <c r="K23">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24">
+        <v>6.3333333333333304</v>
+      </c>
+      <c r="D24">
+        <v>5169.1323166666598</v>
+      </c>
+      <c r="E24">
+        <v>0.17</v>
+      </c>
+      <c r="F24">
+        <v>7.8333333333333304</v>
+      </c>
+      <c r="G24">
+        <v>3931.2337255319098</v>
+      </c>
+      <c r="H24">
+        <v>0.43</v>
+      </c>
+      <c r="I24">
+        <v>5.75</v>
+      </c>
+      <c r="J24">
+        <v>5072.3416956521696</v>
+      </c>
+      <c r="K24">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>8806.6607499999991</v>
+      </c>
+      <c r="E25">
+        <v>0.16</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>55317.168233333301</v>
+      </c>
+      <c r="H25">
+        <v>0.1</v>
+      </c>
+      <c r="I25">
+        <v>0.25</v>
+      </c>
+      <c r="J25">
+        <v>198077.38449999999</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26">
+        <v>4.6666666666666599</v>
+      </c>
+      <c r="D26">
+        <v>5330.3329538461503</v>
+      </c>
+      <c r="E26">
+        <v>0.65</v>
+      </c>
+      <c r="F26">
+        <v>4.3333333333333304</v>
+      </c>
+      <c r="G26">
+        <v>8415.0853269230702</v>
+      </c>
+      <c r="H26">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="I26">
+        <v>3.25</v>
+      </c>
+      <c r="J26">
+        <v>9402.5735846153802</v>
+      </c>
+      <c r="K26">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>32</v>
       </c>

</xml_diff>